<commit_message>
Add MAPPING sheet to Excel spreadsheet
</commit_message>
<xml_diff>
--- a/RJ_Survey0ct2013.xlsx
+++ b/RJ_Survey0ct2013.xlsx
@@ -5,24 +5,24 @@
   <workbookPr date1904="1" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RJones\Documents\Visual Studio 2012\Projects\PythonApplication1\PythonApplication1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UpdateUACMfromExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="495" windowWidth="17895" windowHeight="7485" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="495" windowWidth="17895" windowHeight="7485" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="1" r:id="rId1"/>
     <sheet name="Key" sheetId="2" r:id="rId2"/>
     <sheet name="Export" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Mapping" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3545" uniqueCount="1423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3643" uniqueCount="1493">
   <si>
     <t>V1</t>
   </si>
@@ -3966,18 +3966,12 @@
     <t xml:space="preserve">a ve developed a love for workign with the people of this community.   </t>
   </si>
   <si>
-    <t>WhyDoYouTeach_Part2</t>
-  </si>
-  <si>
     <t xml:space="preserve">I chose to make an ethical decision of discussing the injustice and unethical practices in the school system. Therefore, my choice has resulted in leaving the profession as </t>
   </si>
   <si>
     <t xml:space="preserve"> an early childhood educator. I believe the schools did not want teachers to educate but to perpetuate injustice by teaching to the test.</t>
   </si>
   <si>
-    <t>NT-ReasonForLeaving-Part2</t>
-  </si>
-  <si>
     <t>I have been diagnosed with "wet" macular degeneration.  I have had six procedures over the last 18 months including four operations to try to stop its progression.   This disease causes loss of sharp focus.  This makes it extremely</t>
   </si>
   <si>
@@ -4266,12 +4260,6 @@
     <t>UACM_Candidate_Contact</t>
   </si>
   <si>
-    <t>Phone_Mobile</t>
-  </si>
-  <si>
-    <t>Phone_Other</t>
-  </si>
-  <si>
     <t>WhyDoYouTeach_A</t>
   </si>
   <si>
@@ -4291,6 +4279,228 @@
   </si>
   <si>
     <t>xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx                            xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[UACM_Candidate_Contact] (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [tblRowID]        INT           IDENTITY (1, 1) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [fk_CandidateUID] BIGINT        NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [fk_PantherID]    VARCHAR (15)  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [AddressLine1]    VARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [AddressLine2]    VARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [City]            VARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [State]           VARCHAR (3)   NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Zip]             VARCHAR (15)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Non_GSUEmail]    VARCHAR (100) NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Phone_Mobile]    VARCHAR (16)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Phone_Other]     VARCHAR (16)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [rowTimestamp]    ROWVERSION    NOT NULL,</t>
+  </si>
+  <si>
+    <t>[Non_GSUEmail]</t>
+  </si>
+  <si>
+    <t>[Phone_Mobile]</t>
+  </si>
+  <si>
+    <t>[Phone_Other]</t>
+  </si>
+  <si>
+    <t>[Zip]</t>
+  </si>
+  <si>
+    <t>[City]</t>
+  </si>
+  <si>
+    <t>[State]</t>
+  </si>
+  <si>
+    <t>[AddressLine1]</t>
+  </si>
+  <si>
+    <t>SIZE</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[UACM_Candidate_Data] (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [UniqueID]              BIGINT         IDENTITY (1, 1) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [PantherID]             NVARCHAR (50)  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [CohortNumber]          INT            CONSTRAINT [DF_UACM_Candidate_Data_CohortNumber] DEFAULT ((0)) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [FirstName]             NVARCHAR (50)  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [MiddleName]            NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [LastName]              NVARCHAR (50)  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [NickName]              NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [NameChange]            NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [CertProgram]           NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [CohortYear]            INT            CONSTRAINT [DF_UACM_Candidate_Data_CohortYear] DEFAULT ((0)) NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [SrvAgreement]          BIT            NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [BkgrdCheck]            BIT            NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Insurance]             BIT            CONSTRAINT [DF__UACM_Cand__Insur__3335971A] DEFAULT ((0)) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Race]                  NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Sex]                   NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [DOB]                   SMALLDATETIME  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Eligibilty]            NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Citizenship]           NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [CitizenshipLocation]   NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [ResidentStatus]        NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [ProgramDecision]       NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [ApplicantDecision]     NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [CertificationEligible] NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [CertificationDate]     NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [ESOL_CertEligible]     NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Comment]               NVARCHAR (500) NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Grant_PACT]            BIT            CONSTRAINT [DF__UACM_Cand__Grant__3429BB53] DEFAULT ((0)) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Grant_QuIEL]           BIT            CONSTRAINT [DF__UACM_Cand__Grant__351DDF8C] DEFAULT ((0)) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Grant_3STEMS]          BIT            CONSTRAINT [DF__UACM_Cand__Grant__361203C5] DEFAULT ((0)) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Recruitment1]          NVARCHAR (100) NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Recruitment2]          NVARCHAR (100) NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Recruitment3]          NVARCHAR (100) NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Salutation]            NVARCHAR (5)   NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [EntryGPA]              DECIMAL (4, 3) NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Source]                NVARCHAR (100) NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [ResidentLocation]      NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [rowTimestamp]          ROWVERSION     NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [StatusTag]             NVARCHAR (100) NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [ProgramMasters]        BIT            NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Ethnicity]             NVARCHAR (50)  NULL,</t>
+  </si>
+  <si>
+    <t>UACM_Candidate_Data</t>
+  </si>
+  <si>
+    <t>[PantherID]</t>
+  </si>
+  <si>
+    <t>[LastName]</t>
+  </si>
+  <si>
+    <t>[FirstName]</t>
+  </si>
+  <si>
+    <t>[MiddleName]</t>
+  </si>
+  <si>
+    <t>[MaidenName]</t>
+  </si>
+  <si>
+    <t>[CohortYear]</t>
+  </si>
+  <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>[NameChange]</t>
+  </si>
+  <si>
+    <t>[Alt_Email]</t>
   </si>
 </sst>
 </file>
@@ -4845,7 +5055,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4897,6 +5107,7 @@
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -5246,8 +5457,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BH86"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="AX1" sqref="AX1:AX65536"/>
+    <sheetView topLeftCell="AK1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="AQ24" sqref="AQ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -5286,12 +5497,17 @@
     <col min="35" max="35" width="37.140625" style="4" customWidth="1"/>
     <col min="36" max="36" width="54.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="54.42578125" style="4" customWidth="1"/>
-    <col min="38" max="38" width="8.28515625" style="4" customWidth="1"/>
-    <col min="39" max="39" width="11" style="4" customWidth="1"/>
-    <col min="40" max="44" width="8.85546875" style="4"/>
-    <col min="45" max="45" width="11.140625" style="4" customWidth="1"/>
-    <col min="46" max="46" width="11.28515625" style="4" customWidth="1"/>
-    <col min="47" max="48" width="8.85546875" style="4"/>
+    <col min="38" max="38" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.28515625" style="4" customWidth="1"/>
+    <col min="43" max="43" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.85546875" style="4"/>
     <col min="49" max="49" width="13.28515625" style="4" customWidth="1"/>
     <col min="50" max="50" width="18.85546875" style="4" customWidth="1"/>
     <col min="51" max="51" width="21.85546875" style="4" customWidth="1"/>
@@ -15928,8 +16144,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AY55"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E42" sqref="E33:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17227,8 +17443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AR2" sqref="AR2"/>
+    <sheetView topLeftCell="AH1" workbookViewId="0">
+      <selection sqref="A1:AU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17265,7 +17481,7 @@
   <sheetData>
     <row r="1" spans="1:54" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>1015</v>
@@ -17346,10 +17562,10 @@
         <v>855</v>
       </c>
       <c r="AB1" s="25" t="s">
-        <v>1416</v>
+        <v>1412</v>
       </c>
       <c r="AC1" s="25" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
       <c r="AD1" s="25" t="s">
         <v>856</v>
@@ -17397,16 +17613,16 @@
         <v>869</v>
       </c>
       <c r="AS1" s="26" t="s">
-        <v>1418</v>
+        <v>1414</v>
       </c>
       <c r="AT1" s="26" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
       <c r="AU1" s="26" t="s">
         <v>870</v>
       </c>
       <c r="AV1" s="25" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="AW1" s="25" t="s">
         <v>871</v>
@@ -17429,18 +17645,18 @@
     </row>
     <row r="2" spans="1:54" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>1420</v>
+        <v>1416</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>1421</v>
+        <v>1417</v>
       </c>
       <c r="P2" s="26"/>
       <c r="Q2" s="26"/>
       <c r="AA2" s="25" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
       <c r="AR2" s="25" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
       <c r="AS2" s="26"/>
       <c r="AT2" s="26"/>
@@ -17449,7 +17665,7 @@
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="B3" t="s">
         <v>876</v>
@@ -17569,7 +17785,7 @@
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="B4" t="s">
         <v>878</v>
@@ -17701,7 +17917,7 @@
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="B5" t="s">
         <v>880</v>
@@ -17818,7 +18034,7 @@
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="B6" t="s">
         <v>131</v>
@@ -17938,7 +18154,7 @@
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="B7" t="s">
         <v>882</v>
@@ -18062,12 +18278,12 @@
         <v>0</v>
       </c>
       <c r="BB7" s="27" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="B8" t="s">
         <v>884</v>
@@ -18184,7 +18400,7 @@
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="B9" t="s">
         <v>161</v>
@@ -18313,7 +18529,7 @@
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="B10" t="s">
         <v>888</v>
@@ -18385,7 +18601,7 @@
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="B11" t="s">
         <v>889</v>
@@ -18499,7 +18715,7 @@
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="B12" t="s">
         <v>891</v>
@@ -18607,7 +18823,7 @@
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="B13" t="s">
         <v>893</v>
@@ -18712,7 +18928,7 @@
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="B14" t="s">
         <v>895</v>
@@ -18847,7 +19063,7 @@
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="B15" t="s">
         <v>899</v>
@@ -18988,7 +19204,7 @@
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="B16" t="s">
         <v>900</v>
@@ -19123,7 +19339,7 @@
     </row>
     <row r="17" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="B17" t="s">
         <v>230</v>
@@ -19252,7 +19468,7 @@
     </row>
     <row r="18" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="B18" t="s">
         <v>241</v>
@@ -19378,7 +19594,7 @@
     </row>
     <row r="19" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="B19" t="s">
         <v>905</v>
@@ -19447,7 +19663,7 @@
         <v>1200</v>
       </c>
       <c r="AD19" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="AE19">
         <v>101</v>
@@ -19495,7 +19711,7 @@
     </row>
     <row r="20" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="B20" t="s">
         <v>907</v>
@@ -19615,7 +19831,7 @@
     </row>
     <row r="21" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="B21" t="s">
         <v>908</v>
@@ -19735,7 +19951,7 @@
     </row>
     <row r="22" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="B22" t="s">
         <v>909</v>
@@ -19865,12 +20081,12 @@
         <v>1</v>
       </c>
       <c r="BB22" s="27" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="23" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="B23" t="s">
         <v>912</v>
@@ -19993,7 +20209,7 @@
     </row>
     <row r="24" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="B24" t="s">
         <v>914</v>
@@ -20098,7 +20314,7 @@
     </row>
     <row r="25" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="B25" t="s">
         <v>916</v>
@@ -20197,7 +20413,7 @@
     </row>
     <row r="26" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="B26" t="s">
         <v>301</v>
@@ -20320,7 +20536,7 @@
     </row>
     <row r="27" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="B27" t="s">
         <v>918</v>
@@ -20437,7 +20653,7 @@
     </row>
     <row r="28" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="B28" t="s">
         <v>920</v>
@@ -20557,7 +20773,7 @@
     </row>
     <row r="29" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="B29" t="s">
         <v>324</v>
@@ -20690,12 +20906,12 @@
         <v>1</v>
       </c>
       <c r="BB29" s="27" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="30" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="B30" t="s">
         <v>923</v>
@@ -20806,7 +21022,7 @@
     </row>
     <row r="31" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B31" t="s">
         <v>342</v>
@@ -20923,7 +21139,7 @@
     </row>
     <row r="32" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="B32" t="s">
         <v>926</v>
@@ -21028,7 +21244,7 @@
     </row>
     <row r="33" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="B33" t="s">
         <v>928</v>
@@ -21148,7 +21364,7 @@
     </row>
     <row r="34" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="B34" t="s">
         <v>930</v>
@@ -21259,7 +21475,7 @@
     </row>
     <row r="35" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="B35" t="s">
         <v>932</v>
@@ -21376,7 +21592,7 @@
     </row>
     <row r="36" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="B36" t="s">
         <v>934</v>
@@ -21499,7 +21715,7 @@
     </row>
     <row r="37" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="B37" t="s">
         <v>936</v>
@@ -21625,7 +21841,7 @@
     </row>
     <row r="38" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="B38" t="s">
         <v>399</v>
@@ -21742,7 +21958,7 @@
     </row>
     <row r="39" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="B39" t="s">
         <v>938</v>
@@ -21866,12 +22082,12 @@
         <v>1</v>
       </c>
       <c r="BB39" s="27" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="40" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="B40" t="s">
         <v>417</v>
@@ -21988,7 +22204,7 @@
     </row>
     <row r="41" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="B41" t="s">
         <v>940</v>
@@ -22114,7 +22330,7 @@
     </row>
     <row r="42" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="B42" t="s">
         <v>942</v>
@@ -22192,7 +22408,7 @@
     </row>
     <row r="43" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="B43" t="s">
         <v>944</v>
@@ -22315,7 +22531,7 @@
     </row>
     <row r="44" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="B44" t="s">
         <v>947</v>
@@ -22432,7 +22648,7 @@
     </row>
     <row r="45" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="B45" t="s">
         <v>950</v>
@@ -22546,7 +22762,7 @@
     </row>
     <row r="46" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="B46" t="s">
         <v>459</v>
@@ -22666,7 +22882,7 @@
     </row>
     <row r="47" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="B47" t="s">
         <v>953</v>
@@ -22777,7 +22993,7 @@
     </row>
     <row r="48" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="B48" t="s">
         <v>955</v>
@@ -22846,7 +23062,7 @@
     </row>
     <row r="49" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="B49" t="s">
         <v>957</v>
@@ -22978,7 +23194,7 @@
     </row>
     <row r="50" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="B50" t="s">
         <v>960</v>
@@ -23101,7 +23317,7 @@
     </row>
     <row r="51" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="B51" t="s">
         <v>962</v>
@@ -23230,7 +23446,7 @@
     </row>
     <row r="52" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="B52" t="s">
         <v>964</v>
@@ -23299,7 +23515,7 @@
         <v>1200</v>
       </c>
       <c r="AD52" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="AE52">
         <v>1019</v>
@@ -23353,7 +23569,7 @@
     </row>
     <row r="53" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="B53" t="s">
         <v>510</v>
@@ -23479,7 +23695,7 @@
     </row>
     <row r="54" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="B54" t="s">
         <v>966</v>
@@ -23605,7 +23821,7 @@
     </row>
     <row r="55" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="B55" t="s">
         <v>969</v>
@@ -23689,7 +23905,7 @@
     </row>
     <row r="56" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="B56" t="s">
         <v>971</v>
@@ -23812,7 +24028,7 @@
     </row>
     <row r="57" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="B57" t="s">
         <v>974</v>
@@ -23929,7 +24145,7 @@
     </row>
     <row r="58" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="B58" t="s">
         <v>976</v>
@@ -24048,7 +24264,7 @@
     </row>
     <row r="59" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="B59" t="s">
         <v>978</v>
@@ -24165,15 +24381,15 @@
         <v>551</v>
       </c>
       <c r="AU59" s="27" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="AV59" s="28" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="60" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="B60" t="s">
         <v>555</v>
@@ -24287,12 +24503,12 @@
         <v>1</v>
       </c>
       <c r="BB60" s="27" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="61" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="B61" t="s">
         <v>980</v>
@@ -24412,7 +24628,7 @@
     </row>
     <row r="62" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="B62" t="s">
         <v>983</v>
@@ -24532,7 +24748,7 @@
     </row>
     <row r="63" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="B63" t="s">
         <v>985</v>
@@ -24655,7 +24871,7 @@
     </row>
     <row r="64" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="B64" t="s">
         <v>586</v>
@@ -24775,7 +24991,7 @@
     </row>
     <row r="65" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="B65" t="s">
         <v>988</v>
@@ -24899,12 +25115,12 @@
         <v>1</v>
       </c>
       <c r="BB65" s="27" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="66" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="B66" t="s">
         <v>605</v>
@@ -25021,7 +25237,7 @@
     </row>
     <row r="67" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="B67" t="s">
         <v>991</v>
@@ -25129,7 +25345,7 @@
     </row>
     <row r="68" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="B68" t="s">
         <v>619</v>
@@ -25258,7 +25474,7 @@
     </row>
     <row r="69" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="B69" t="s">
         <v>631</v>
@@ -25372,7 +25588,7 @@
     </row>
     <row r="70" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="B70" t="s">
         <v>882</v>
@@ -25486,7 +25702,7 @@
     </row>
     <row r="71" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="B71" t="s">
         <v>996</v>
@@ -25603,7 +25819,7 @@
     </row>
     <row r="72" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="B72" t="s">
         <v>998</v>
@@ -25726,7 +25942,7 @@
     </row>
     <row r="73" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="B73" t="s">
         <v>1000</v>
@@ -25847,12 +26063,12 @@
         <v>1</v>
       </c>
       <c r="BB73" s="27" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="74" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="B74" t="s">
         <v>1002</v>
@@ -25966,7 +26182,7 @@
     </row>
     <row r="75" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="B75" t="s">
         <v>161</v>
@@ -26086,7 +26302,7 @@
     </row>
     <row r="76" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="B76" t="s">
         <v>1005</v>
@@ -26206,7 +26422,7 @@
     </row>
     <row r="77" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="B77" t="s">
         <v>1007</v>
@@ -26299,7 +26515,7 @@
     </row>
     <row r="78" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="B78" t="s">
         <v>605</v>
@@ -26422,7 +26638,7 @@
     </row>
     <row r="79" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="B79" t="s">
         <v>1009</v>
@@ -26539,10 +26755,10 @@
         <v>716</v>
       </c>
       <c r="AS79" s="27" t="s">
+        <v>1314</v>
+      </c>
+      <c r="AT79" s="27" t="s">
         <v>1315</v>
-      </c>
-      <c r="AT79" s="27" t="s">
-        <v>1316</v>
       </c>
       <c r="AU79" s="27" t="s">
         <v>717</v>
@@ -26569,7 +26785,7 @@
     </row>
     <row r="80" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="B80" t="s">
         <v>722</v>
@@ -26674,7 +26890,7 @@
     </row>
     <row r="81" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="B81" t="s">
         <v>1013</v>
@@ -26821,10 +27037,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26832,268 +27048,607 @@
     <col min="1" max="1" width="30.5703125" customWidth="1"/>
     <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C1" t="s">
         <v>1410</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>1441</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1485</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1486</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1487</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>1488</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1491</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>840</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1489</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1490</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1490</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1490</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1490</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B13" t="s">
         <v>1411</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C13" t="s">
+        <v>1438</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E13">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>842</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>843</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1432</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>844</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>1492</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>846</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>847</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="25" t="s">
+        <v>848</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>849</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
+        <v>851</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
+        <v>852</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
+        <v>854</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="25" t="s">
+        <v>855</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
         <v>1412</v>
       </c>
+      <c r="G29" t="s">
+        <v>1454</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>1016</v>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="25" t="s">
+        <v>1413</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1455</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>1017</v>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>856</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1456</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>1307</v>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
+        <v>1305</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1457</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>1022</v>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="25" t="s">
+        <v>857</v>
+      </c>
+      <c r="C33" t="s">
+        <v>804</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1458</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>840</v>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>858</v>
+      </c>
+      <c r="C34" t="s">
+        <v>804</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1459</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>1308</v>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="25" t="s">
+        <v>859</v>
+      </c>
+      <c r="C35" t="s">
+        <v>804</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1460</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>54</v>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
+        <v>860</v>
+      </c>
+      <c r="C36" t="s">
+        <v>804</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1461</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>1306</v>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="25" t="s">
+        <v>861</v>
+      </c>
+      <c r="C37" t="s">
+        <v>805</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1462</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>1309</v>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="25" t="s">
+        <v>862</v>
+      </c>
+      <c r="C38" t="s">
+        <v>805</v>
+      </c>
+      <c r="G38" t="s">
+        <v>1463</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>1190</v>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="25" t="s">
+        <v>863</v>
+      </c>
+      <c r="C39" t="s">
+        <v>805</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1464</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>1191</v>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="25" t="s">
+        <v>864</v>
+      </c>
+      <c r="C40" t="s">
+        <v>805</v>
+      </c>
+      <c r="G40" t="s">
+        <v>1465</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>1192</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1413</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1192</v>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
+        <v>865</v>
+      </c>
+      <c r="C41" t="s">
+        <v>805</v>
+      </c>
+      <c r="G41" t="s">
+        <v>1466</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
-        <v>1193</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1413</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1193</v>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="25" t="s">
+        <v>866</v>
+      </c>
+      <c r="C42" t="s">
+        <v>806</v>
+      </c>
+      <c r="G42" t="s">
+        <v>1467</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>1177</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1413</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1177</v>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
+        <v>867</v>
+      </c>
+      <c r="G43" t="s">
+        <v>1468</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>842</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1413</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
+        <v>868</v>
+      </c>
+      <c r="G44" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="26" t="s">
+        <v>869</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="26" t="s">
+        <v>1414</v>
+      </c>
+      <c r="G46" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="26" t="s">
         <v>1415</v>
       </c>
+      <c r="G47" t="s">
+        <v>1472</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>843</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1413</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1414</v>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="26" t="s">
+        <v>870</v>
+      </c>
+      <c r="G48" t="s">
+        <v>1473</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1413</v>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>1474</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
-        <v>844</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1413</v>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>1475</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>846</v>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>1476</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>847</v>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>1477</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
-        <v>848</v>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>1478</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
-        <v>849</v>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>1479</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
-        <v>851</v>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>1480</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>852</v>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>1481</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
-        <v>1314</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
-        <v>1305</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
-        <v>1317</v>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>1482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>